<commit_message>
Update BienBanHopVaLamViec + Video
</commit_message>
<xml_diff>
--- a/Documents/1603223_FIT_LinkVideoMinhChung.xlsx
+++ b/Documents/1603223_FIT_LinkVideoMinhChung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY GIT\DUAN1\TTCSN-GROUP10\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY GIT\DUAN1\TTCSN-GROUP10\BaoCao\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FB0092-9DF4-41E6-BB28-08DA24EBA7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0485AB7D-0AD8-4CC0-B1BB-8486DB6A6E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2592" yWindow="1548" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>https://www.youtube.com/watch?v=PP9UjVCCzKU&amp;t=34s</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>https://youtu.be/UyXkte02GQQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/d8Ub1Z0KhAc</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -495,12 +500,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>